<commit_message>
Results for GraphSAGE supervised.
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333A3162-3365-4BAB-ACB2-D3F4A1A0EC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A142E321-EA5D-455A-B0B3-E0B06C27A039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GraphSAGE+XGBoost" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="27">
   <si>
     <t>Dimension</t>
   </si>
@@ -85,6 +85,27 @@
   <si>
     <t>n2v</t>
   </si>
+  <si>
+    <t>gcn_small_0.0100</t>
+  </si>
+  <si>
+    <t>Loss</t>
+  </si>
+  <si>
+    <t>F1_Micro</t>
+  </si>
+  <si>
+    <t>F1_Macro</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Val</t>
+  </si>
+  <si>
+    <t>Test_or_Val</t>
+  </si>
 </sst>
 </file>
 
@@ -119,10 +140,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -404,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,7 +444,7 @@
     <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -439,8 +463,11 @@
       <c r="F1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -459,8 +486,11 @@
       <c r="F2" s="1">
         <v>0.14509629642118199</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -479,8 +509,11 @@
       <c r="F3" s="1">
         <v>0.283849053654674</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -499,8 +532,11 @@
       <c r="F4" s="1">
         <v>0.36578420457227001</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -519,8 +555,11 @@
       <c r="F5" s="1">
         <v>0.37534648498300699</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -539,8 +578,11 @@
       <c r="F6" s="1">
         <v>0.42627483949109302</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -558,6 +600,9 @@
       </c>
       <c r="F7" s="1">
         <v>3.1048105664610798E-3</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -567,12 +612,243 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.30408000000000002</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.85487999999999997</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.48658000000000001</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.23588999999999999</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.88771</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.70133999999999996</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.24249999999999999</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.89446000000000003</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.75022999999999995</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.21962000000000001</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.90105999999999997</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.75531000000000004</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.23255000000000001</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.90237000000000001</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.77325999999999995</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.32694000000000001</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.85348999999999997</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.48638999999999999</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.2477</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.88097000000000003</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.69376000000000004</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.24138999999999999</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.90456999999999999</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.77881</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.21364</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.91056000000000004</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.78483000000000003</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.22484000000000001</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.90859999999999996</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.78715000000000002</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -581,7 +857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J264"/>
   <sheetViews>
-    <sheetView topLeftCell="A186" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A264" sqref="A264"/>
     </sheetView>
   </sheetViews>
@@ -9070,7 +9346,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>